<commit_message>
Modify distance recht border
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssbb_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssbb_vorlage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws-intern\PlanPro-Git\eclipse-set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68D6862-11C7-4EC1-A6F4-03D6A1ACBE24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9FC0E7-215A-4484-82D5-78B58A2B25C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1221,17 +1221,13 @@
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="E3:G3"/>
   </mergeCells>
-  <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.19685039370078741" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.19685039370078741" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1240,53 +1236,11 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fb340e34ecc5d059b634082484788e96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae5cd419a40dc0c21009e0c04d2bd83e" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -1478,7 +1432,61 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B177577A-2CEE-43F9-AC4C-E98CE9889969}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCCD530F-547F-4AD6-854B-33238E773658}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
@@ -1486,23 +1494,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B177577A-2CEE-43F9-AC4C-E98CE9889969}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{178C0AFF-C5EC-49D6-8ED9-EFFBD8AEB2DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{513029CE-D345-43C7-867C-30BD796A1540}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1519,4 +1511,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{178C0AFF-C5EC-49D6-8ED9-EFFBD8AEB2DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Table Export : Modify right margin (#1071)
* Modify distance recht border

* add comment, change variable name

* Fix table width by multipage
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssbb_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssbb_vorlage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws-intern\PlanPro-Git\eclipse-set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68D6862-11C7-4EC1-A6F4-03D6A1ACBE24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9FC0E7-215A-4484-82D5-78B58A2B25C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1221,17 +1221,13 @@
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="E3:G3"/>
   </mergeCells>
-  <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.19685039370078741" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.19685039370078741" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1240,53 +1236,11 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fb340e34ecc5d059b634082484788e96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae5cd419a40dc0c21009e0c04d2bd83e" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -1478,7 +1432,61 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B177577A-2CEE-43F9-AC4C-E98CE9889969}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCCD530F-547F-4AD6-854B-33238E773658}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
@@ -1486,23 +1494,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B177577A-2CEE-43F9-AC4C-E98CE9889969}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{178C0AFF-C5EC-49D6-8ED9-EFFBD8AEB2DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{513029CE-D345-43C7-867C-30BD796A1540}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1519,4 +1511,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{178C0AFF-C5EC-49D6-8ED9-EFFBD8AEB2DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix table border by export
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssbb_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssbb_vorlage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws-intern\PlanPro-Git\eclipse-set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws_intern\planpro\set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9FC0E7-215A-4484-82D5-78B58A2B25C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C78DE0-C0EE-4B8F-A161-D0F6FB23FE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ssbb_Beispielbefüllung" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -249,112 +249,71 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -362,28 +321,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -395,108 +338,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -518,9 +437,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -558,9 +477,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -593,26 +512,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -645,26 +547,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -838,382 +723,322 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K62"/>
+  <dimension ref="B1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="17" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="17" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="17" customWidth="1"/>
-    <col min="9" max="10" width="13.42578125" style="17" customWidth="1"/>
-    <col min="11" max="11" width="75.85546875" style="21" customWidth="1"/>
-    <col min="12" max="12" width="25.5703125" style="17" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="17"/>
+    <col min="1" max="1" width="3.28515625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="10" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="10" customWidth="1"/>
+    <col min="9" max="10" width="13.42578125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="75.85546875" style="11" customWidth="1"/>
+    <col min="12" max="12" width="25.5703125" style="10" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="2:11" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="9" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="29" t="s">
+    <row r="2" spans="2:11" s="1" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="29" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="15" t="s">
+      <c r="I2" s="22"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="9" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="11" t="s">
+    <row r="3" spans="2:11" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="8" t="s">
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="18"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="2:11" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="19"/>
-    </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="17"/>
+    </row>
+    <row r="5" spans="2:11" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="4"/>
       <c r="I5" s="3"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="20"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="25"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="28"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="K8" s="17"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="K9" s="17"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="K10" s="17"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="K11" s="17"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="K12" s="17"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="K13" s="17"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="K14" s="17"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="K15" s="17"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="K16" s="17"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="K17" s="17"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="K18" s="17"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="K19" s="17"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="K20" s="17"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="K21" s="17"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="K22" s="17"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="K23" s="17"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="K24" s="17"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="K25" s="17"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="K26" s="17"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="K27" s="17"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="K28" s="17"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="K29" s="17"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="K30" s="17"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="K31" s="17"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="K32" s="17"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="K33" s="17"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-      <c r="K34" s="17"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-      <c r="K35" s="17"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="K36" s="17"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="K37" s="17"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="K38" s="17"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="K39" s="17"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="K40" s="17"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="K41" s="17"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="K42" s="17"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
-      <c r="K43" s="17"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
-      <c r="K44" s="17"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
-      <c r="K45" s="17"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
-      <c r="K46" s="17"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
-      <c r="K47" s="17"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
-      <c r="K48" s="17"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
-      <c r="K49" s="17"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-      <c r="K50" s="17"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
-      <c r="K51" s="17"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="17"/>
-      <c r="K52" s="17"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="17"/>
-      <c r="K53" s="17"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="K54" s="17"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-      <c r="K55" s="17"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="17"/>
-      <c r="K56" s="17"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="17"/>
-      <c r="K57" s="17"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="17"/>
-      <c r="K58" s="17"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="17"/>
-      <c r="K59" s="17"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="17"/>
-      <c r="K60" s="17"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="17"/>
-      <c r="K61" s="17"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="17"/>
-      <c r="K62" s="17"/>
+      <c r="K5" s="18"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="13"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="13"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="10"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="10"/>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="10"/>
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="10"/>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="10"/>
+    </row>
+    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="10"/>
+    </row>
+    <row r="22" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="10"/>
+    </row>
+    <row r="23" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="10"/>
+    </row>
+    <row r="24" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="10"/>
+    </row>
+    <row r="25" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="10"/>
+    </row>
+    <row r="26" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="10"/>
+    </row>
+    <row r="27" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="10"/>
+    </row>
+    <row r="28" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K28" s="10"/>
+    </row>
+    <row r="29" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K29" s="10"/>
+    </row>
+    <row r="30" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K30" s="10"/>
+    </row>
+    <row r="31" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K31" s="10"/>
+    </row>
+    <row r="32" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K32" s="10"/>
+    </row>
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K33" s="10"/>
+    </row>
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K34" s="10"/>
+    </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K35" s="10"/>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="10"/>
+    </row>
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K37" s="10"/>
+    </row>
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="10"/>
+    </row>
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K39" s="10"/>
+    </row>
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K40" s="10"/>
+    </row>
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K41" s="10"/>
+    </row>
+    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K42" s="10"/>
+    </row>
+    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K43" s="10"/>
+    </row>
+    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K44" s="10"/>
+    </row>
+    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K45" s="10"/>
+    </row>
+    <row r="46" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K46" s="10"/>
+    </row>
+    <row r="47" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K47" s="10"/>
+    </row>
+    <row r="48" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K48" s="10"/>
+    </row>
+    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K49" s="10"/>
+    </row>
+    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K50" s="10"/>
+    </row>
+    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K51" s="10"/>
+    </row>
+    <row r="52" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K52" s="10"/>
+    </row>
+    <row r="53" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K53" s="10"/>
+    </row>
+    <row r="54" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K54" s="10"/>
+    </row>
+    <row r="55" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K55" s="10"/>
+    </row>
+    <row r="56" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K56" s="10"/>
+    </row>
+    <row r="57" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K57" s="10"/>
+    </row>
+    <row r="58" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K58" s="10"/>
+    </row>
+    <row r="59" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K59" s="10"/>
+    </row>
+    <row r="60" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K60" s="10"/>
+    </row>
+    <row r="61" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K61" s="10"/>
+    </row>
+    <row r="62" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K62" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Fix table border by export (#1789)
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssbb_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssbb_vorlage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws-intern\PlanPro-Git\eclipse-set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws_intern\planpro\set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9FC0E7-215A-4484-82D5-78B58A2B25C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C78DE0-C0EE-4B8F-A161-D0F6FB23FE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ssbb_Beispielbefüllung" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -249,112 +249,71 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -362,28 +321,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -395,108 +338,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -518,9 +437,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -558,9 +477,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -593,26 +512,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -645,26 +547,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -838,382 +723,322 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K62"/>
+  <dimension ref="B1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="17" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="17" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="17" customWidth="1"/>
-    <col min="9" max="10" width="13.42578125" style="17" customWidth="1"/>
-    <col min="11" max="11" width="75.85546875" style="21" customWidth="1"/>
-    <col min="12" max="12" width="25.5703125" style="17" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="17"/>
+    <col min="1" max="1" width="3.28515625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="10" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="10" customWidth="1"/>
+    <col min="9" max="10" width="13.42578125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="75.85546875" style="11" customWidth="1"/>
+    <col min="12" max="12" width="25.5703125" style="10" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="2:11" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="9" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="29" t="s">
+    <row r="2" spans="2:11" s="1" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="29" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="15" t="s">
+      <c r="I2" s="22"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="9" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="11" t="s">
+    <row r="3" spans="2:11" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="8" t="s">
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="18"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="2:11" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="19"/>
-    </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="17"/>
+    </row>
+    <row r="5" spans="2:11" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="4"/>
       <c r="I5" s="3"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="20"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="25"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="28"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="K8" s="17"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="K9" s="17"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="K10" s="17"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="K11" s="17"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="K12" s="17"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="K13" s="17"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="K14" s="17"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="K15" s="17"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="K16" s="17"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="K17" s="17"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="K18" s="17"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="K19" s="17"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="K20" s="17"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="K21" s="17"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="K22" s="17"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="K23" s="17"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="K24" s="17"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="K25" s="17"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="K26" s="17"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="K27" s="17"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="K28" s="17"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="K29" s="17"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="K30" s="17"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="K31" s="17"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="K32" s="17"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="K33" s="17"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-      <c r="K34" s="17"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-      <c r="K35" s="17"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="K36" s="17"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="K37" s="17"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="K38" s="17"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="K39" s="17"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="K40" s="17"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="K41" s="17"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="K42" s="17"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
-      <c r="K43" s="17"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
-      <c r="K44" s="17"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
-      <c r="K45" s="17"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
-      <c r="K46" s="17"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
-      <c r="K47" s="17"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
-      <c r="K48" s="17"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
-      <c r="K49" s="17"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-      <c r="K50" s="17"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
-      <c r="K51" s="17"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="17"/>
-      <c r="K52" s="17"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="17"/>
-      <c r="K53" s="17"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="K54" s="17"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-      <c r="K55" s="17"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="17"/>
-      <c r="K56" s="17"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="17"/>
-      <c r="K57" s="17"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="17"/>
-      <c r="K58" s="17"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="17"/>
-      <c r="K59" s="17"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="17"/>
-      <c r="K60" s="17"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="17"/>
-      <c r="K61" s="17"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="17"/>
-      <c r="K62" s="17"/>
+      <c r="K5" s="18"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="13"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="13"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="10"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="10"/>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="10"/>
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="10"/>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="10"/>
+    </row>
+    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="10"/>
+    </row>
+    <row r="22" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="10"/>
+    </row>
+    <row r="23" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="10"/>
+    </row>
+    <row r="24" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="10"/>
+    </row>
+    <row r="25" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="10"/>
+    </row>
+    <row r="26" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="10"/>
+    </row>
+    <row r="27" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="10"/>
+    </row>
+    <row r="28" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K28" s="10"/>
+    </row>
+    <row r="29" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K29" s="10"/>
+    </row>
+    <row r="30" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K30" s="10"/>
+    </row>
+    <row r="31" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K31" s="10"/>
+    </row>
+    <row r="32" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K32" s="10"/>
+    </row>
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K33" s="10"/>
+    </row>
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K34" s="10"/>
+    </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K35" s="10"/>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="10"/>
+    </row>
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K37" s="10"/>
+    </row>
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="10"/>
+    </row>
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K39" s="10"/>
+    </row>
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K40" s="10"/>
+    </row>
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K41" s="10"/>
+    </row>
+    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K42" s="10"/>
+    </row>
+    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K43" s="10"/>
+    </row>
+    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K44" s="10"/>
+    </row>
+    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K45" s="10"/>
+    </row>
+    <row r="46" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K46" s="10"/>
+    </row>
+    <row r="47" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K47" s="10"/>
+    </row>
+    <row r="48" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K48" s="10"/>
+    </row>
+    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K49" s="10"/>
+    </row>
+    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K50" s="10"/>
+    </row>
+    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K51" s="10"/>
+    </row>
+    <row r="52" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K52" s="10"/>
+    </row>
+    <row r="53" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K53" s="10"/>
+    </row>
+    <row r="54" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K54" s="10"/>
+    </row>
+    <row r="55" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K55" s="10"/>
+    </row>
+    <row r="56" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K56" s="10"/>
+    </row>
+    <row r="57" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K57" s="10"/>
+    </row>
+    <row r="58" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K58" s="10"/>
+    </row>
+    <row r="59" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K59" s="10"/>
+    </row>
+    <row r="60" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K60" s="10"/>
+    </row>
+    <row r="61" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K61" s="10"/>
+    </row>
+    <row r="62" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K62" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>